<commit_message>
Opdelen fairness anayze code
</commit_message>
<xml_diff>
--- a/scripts/dev/mapping_1cho.xlsx
+++ b/scripts/dev/mapping_1cho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahtanjung/Projects/ceda-fairnessawareness/scripts/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36093DD7-29E7-D443-9C01-0BF18A50DF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56AC0CF-8BDB-1C4E-9EA5-288F5FF862E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{B78D59E7-0030-0645-8726-42CC1661625F}"/>
   </bookViews>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451CCA4F-1413-6B47-897A-0B7E340EE5BC}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>